<commit_message>
Add Tesis reformat and more things
</commit_message>
<xml_diff>
--- a/Calculos Excel/Viabilidad economica.xlsx
+++ b/Calculos Excel/Viabilidad economica.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b6fe671ebe24109/Tesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Tesis_bi_microclin\Calculos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="884" documentId="13_ncr:1_{1A0BAA6E-3867-4400-BDD4-3D00522DDC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B28BA1F-9189-4A8B-97AA-B1D19C51B744}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7781C5D5-5CCF-45A5-A014-225258FFE43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Viabilidad economica" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -282,9 +283,6 @@
     <t>Costo (S/.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiempo </t>
-  </si>
-  <si>
     <t>Asesoría Trimestral (Ingeniero de sistemas)</t>
   </si>
   <si>
@@ -349,9 +347,6 @@
   </si>
   <si>
     <t>Monto (S/. Año)</t>
-  </si>
-  <si>
-    <t>Ahorro por reducción de personal</t>
   </si>
   <si>
     <t>Flujo de Caja</t>
@@ -479,17 +474,23 @@
   <si>
     <t>VAN</t>
   </si>
+  <si>
+    <t xml:space="preserve">Frecuencia </t>
+  </si>
+  <si>
+    <t>Reducción y ahorros</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-&quot;S/&quot;\ * #,##0.00_-;\-&quot;S/&quot;\ * #,##0.00_-;_-&quot;S/&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@"/>
-    <numFmt numFmtId="167" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;\ * #,##0.00_-;\-&quot;S/&quot;\ * #,##0.00_-;_-&quot;S/&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@"/>
+    <numFmt numFmtId="168" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -624,7 +625,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -651,19 +652,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAEAAAA"/>
-        <bgColor rgb="FFAEAAAA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,9 +830,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -855,7 +844,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -877,9 +866,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -895,7 +881,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -905,8 +890,8 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,16 +905,13 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -942,14 +924,73 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -958,58 +999,77 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1022,109 +1082,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1132,18 +1129,12 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1379,9 +1370,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>-85725</xdr:rowOff>
+      <xdr:colOff>55162</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>78022</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4029075" cy="2790825"/>
     <xdr:pic>
@@ -1402,6 +1393,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792314" y="22590152"/>
+          <a:ext cx="4029075" cy="2790825"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1554,8 +1549,8 @@
       <xdr:rowOff>74544</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3230880" cy="431657"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CuadroTexto 31">
@@ -1807,19 +1802,7 @@
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
-                                  <m:t>(</m:t>
-                                </m:r>
-                                <m:r>
-                                  <a:rPr lang="es-MX" sz="1100">
-                                    <a:solidFill>
-                                      <a:schemeClr val="tx1"/>
-                                    </a:solidFill>
-                                    <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
-                                    <a:ea typeface="+mn-ea"/>
-                                    <a:cs typeface="+mn-cs"/>
-                                  </a:rPr>
-                                  <m:t>1+</m:t>
+                                  <m:t>(1+</m:t>
                                 </m:r>
                                 <m:r>
                                   <a:rPr lang="es-MX" sz="1100" b="0" i="0">
@@ -1827,7 +1810,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1950,19 +1933,7 @@
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
-                                  <m:t>(</m:t>
-                                </m:r>
-                                <m:r>
-                                  <a:rPr lang="es-MX" sz="1100">
-                                    <a:solidFill>
-                                      <a:schemeClr val="tx1"/>
-                                    </a:solidFill>
-                                    <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
-                                    <a:ea typeface="+mn-ea"/>
-                                    <a:cs typeface="+mn-cs"/>
-                                  </a:rPr>
-                                  <m:t>1+</m:t>
+                                  <m:t>(1+</m:t>
                                 </m:r>
                                 <m:r>
                                   <a:rPr lang="es-MX" sz="1100" b="0" i="0">
@@ -1970,7 +1941,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2016,7 +1987,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CuadroTexto 31">
@@ -2441,8 +2412,8 @@
       <xdr:rowOff>17890</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1297374" cy="214023"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="39" name="CuadroTexto 32">
@@ -2537,7 +2508,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="39" name="CuadroTexto 32">
@@ -2967,8 +2938,8 @@
       <xdr:rowOff>31225</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3795346" cy="431657"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="57" name="CuadroTexto 34">
@@ -3161,7 +3132,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -3289,7 +3260,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -3417,7 +3388,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -3468,7 +3439,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="57" name="CuadroTexto 34">
@@ -9008,8 +8979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L152" sqref="L152"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9056,13 +9027,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -9114,10 +9085,10 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="75"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -9144,10 +9115,10 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="54"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -9174,21 +9145,21 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="62"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="62"/>
+      <c r="H6" s="55"/>
       <c r="I6" s="3" t="s">
         <v>7</v>
       </c>
@@ -9212,22 +9183,22 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="87" t="s">
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="60">
         <v>1</v>
       </c>
-      <c r="G7" s="90">
+      <c r="G7" s="89">
         <v>4200</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="91">
+      <c r="H7" s="72"/>
+      <c r="I7" s="90">
         <f>G7*F7</f>
         <v>4200</v>
       </c>
@@ -9251,14 +9222,14 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="49"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="57"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -9279,22 +9250,22 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="87" t="s">
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F9" s="60">
         <v>1</v>
       </c>
-      <c r="G9" s="90">
+      <c r="G9" s="89">
         <v>3800</v>
       </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="91">
+      <c r="H9" s="72"/>
+      <c r="I9" s="90">
         <f>G9*F9</f>
         <v>3800</v>
       </c>
@@ -9318,14 +9289,14 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="49"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="57"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -9346,22 +9317,22 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="87" t="s">
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="48">
+      <c r="F11" s="60">
         <v>1</v>
       </c>
-      <c r="G11" s="90">
+      <c r="G11" s="89">
         <v>720</v>
       </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="91">
+      <c r="H11" s="72"/>
+      <c r="I11" s="90">
         <f>G11*F11</f>
         <v>720</v>
       </c>
@@ -9385,14 +9356,14 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="49"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="57"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -9413,25 +9384,25 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="22">
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="20">
         <f>I7+I9+I11</f>
         <v>8720</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="70" t="s">
+      <c r="K13" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -9457,10 +9428,10 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="83" t="s">
+      <c r="K14" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="62"/>
+      <c r="L14" s="55"/>
       <c r="M14" s="3" t="s">
         <v>7</v>
       </c>
@@ -9480,10 +9451,10 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -9491,11 +9462,11 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="60" t="s">
+      <c r="K15" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="62"/>
-      <c r="M15" s="23">
+      <c r="L15" s="55"/>
+      <c r="M15" s="21">
         <f>I13</f>
         <v>8720</v>
       </c>
@@ -9515,29 +9486,29 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="83" t="s">
+      <c r="B16" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="62"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="84" t="s">
+      <c r="G16" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="62"/>
+      <c r="H16" s="55"/>
       <c r="I16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="60" t="s">
+      <c r="K16" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="62"/>
+      <c r="L16" s="55"/>
       <c r="M16" s="12">
         <f>I26</f>
         <v>0</v>
@@ -9558,30 +9529,30 @@
     </row>
     <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="62"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="22">
         <v>2</v>
       </c>
-      <c r="G17" s="89">
+      <c r="G17" s="94">
         <v>0</v>
       </c>
-      <c r="H17" s="62"/>
+      <c r="H17" s="55"/>
       <c r="I17" s="12">
         <v>0</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="92" t="s">
+      <c r="K17" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="62"/>
-      <c r="M17" s="25">
+      <c r="L17" s="55"/>
+      <c r="M17" s="23">
         <f>M15+M16</f>
         <v>8720</v>
       </c>
@@ -9601,21 +9572,21 @@
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="22">
         <v>2</v>
       </c>
-      <c r="G18" s="88">
+      <c r="G18" s="81">
         <v>0</v>
       </c>
-      <c r="H18" s="62"/>
+      <c r="H18" s="55"/>
       <c r="I18" s="12">
         <v>0</v>
       </c>
@@ -9639,21 +9610,21 @@
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="22">
         <v>2</v>
       </c>
-      <c r="G19" s="88">
+      <c r="G19" s="81">
         <v>0</v>
       </c>
-      <c r="H19" s="62"/>
+      <c r="H19" s="55"/>
       <c r="I19" s="12">
         <v>0</v>
       </c>
@@ -9677,21 +9648,21 @@
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="22">
         <v>2</v>
       </c>
-      <c r="G20" s="88">
+      <c r="G20" s="81">
         <v>0</v>
       </c>
-      <c r="H20" s="62"/>
+      <c r="H20" s="55"/>
       <c r="I20" s="12">
         <v>0</v>
       </c>
@@ -9715,21 +9686,21 @@
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="22">
         <v>2</v>
       </c>
-      <c r="G21" s="88">
+      <c r="G21" s="81">
         <v>0</v>
       </c>
-      <c r="H21" s="62"/>
+      <c r="H21" s="55"/>
       <c r="I21" s="12">
         <v>0</v>
       </c>
@@ -9753,21 +9724,21 @@
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="22">
         <v>2</v>
       </c>
-      <c r="G22" s="88">
+      <c r="G22" s="81">
         <v>0</v>
       </c>
-      <c r="H22" s="62"/>
+      <c r="H22" s="55"/>
       <c r="I22" s="12">
         <v>0</v>
       </c>
@@ -9791,21 +9762,21 @@
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="62"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="22">
         <v>2</v>
       </c>
-      <c r="G23" s="88">
+      <c r="G23" s="81">
         <v>0</v>
       </c>
-      <c r="H23" s="62"/>
+      <c r="H23" s="55"/>
       <c r="I23" s="12">
         <v>0</v>
       </c>
@@ -9829,21 +9800,21 @@
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="24">
+      <c r="F24" s="22">
         <v>2</v>
       </c>
-      <c r="G24" s="88">
+      <c r="G24" s="81">
         <v>0</v>
       </c>
-      <c r="H24" s="62"/>
+      <c r="H24" s="55"/>
       <c r="I24" s="12">
         <v>0</v>
       </c>
@@ -9867,21 +9838,21 @@
     </row>
     <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="62"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
       <c r="E25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="22">
         <v>2</v>
       </c>
-      <c r="G25" s="88">
+      <c r="G25" s="81">
         <v>0</v>
       </c>
-      <c r="H25" s="62"/>
+      <c r="H25" s="55"/>
       <c r="I25" s="12">
         <v>0</v>
       </c>
@@ -9905,16 +9876,16 @@
     </row>
     <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="26">
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="24">
         <v>0</v>
       </c>
       <c r="J26" s="1"/>
@@ -9965,10 +9936,10 @@
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="75"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -9995,10 +9966,10 @@
     </row>
     <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -10025,20 +9996,20 @@
     </row>
     <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="62"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="83" t="s">
+      <c r="F30" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="62"/>
+      <c r="G30" s="55"/>
       <c r="H30" s="5" t="s">
         <v>7</v>
       </c>
@@ -10063,23 +10034,23 @@
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="62"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="12">
         <v>2</v>
       </c>
       <c r="E31" s="12">
-        <v>4</v>
-      </c>
-      <c r="F31" s="81">
+        <v>2.75</v>
+      </c>
+      <c r="F31" s="96">
         <v>1025</v>
       </c>
-      <c r="G31" s="62"/>
-      <c r="H31" s="27">
+      <c r="G31" s="55"/>
+      <c r="H31" s="25">
         <f>F31*D31*E31</f>
-        <v>8200</v>
+        <v>5637.5</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -10102,17 +10073,17 @@
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="82" t="s">
+      <c r="B32" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="28">
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="26">
         <f>H31</f>
-        <v>8200</v>
+        <v>5637.5</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -10163,10 +10134,10 @@
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="47"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -10193,20 +10164,20 @@
     </row>
     <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="83" t="s">
+      <c r="B35" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="62"/>
+      <c r="C35" s="55"/>
       <c r="D35" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="83" t="s">
+      <c r="F35" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="62"/>
+      <c r="G35" s="55"/>
       <c r="H35" s="3" t="s">
         <v>18</v>
       </c>
@@ -10231,21 +10202,21 @@
     </row>
     <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="62"/>
+      <c r="C36" s="55"/>
       <c r="D36" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="22">
         <v>1</v>
       </c>
-      <c r="F36" s="80">
+      <c r="F36" s="95">
         <v>16</v>
       </c>
-      <c r="G36" s="62"/>
-      <c r="H36" s="24">
+      <c r="G36" s="55"/>
+      <c r="H36" s="22">
         <f t="shared" ref="H36:H42" si="0">F36*E36</f>
         <v>16</v>
       </c>
@@ -10272,29 +10243,29 @@
     </row>
     <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="62"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E37" s="22">
         <v>5</v>
       </c>
-      <c r="F37" s="80">
+      <c r="F37" s="95">
         <v>0.8</v>
       </c>
-      <c r="G37" s="62"/>
-      <c r="H37" s="24">
+      <c r="G37" s="55"/>
+      <c r="H37" s="22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I37" s="29"/>
-      <c r="J37" s="84" t="s">
+      <c r="I37" s="27"/>
+      <c r="J37" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="62"/>
+      <c r="K37" s="55"/>
       <c r="L37" s="8" t="s">
         <v>40</v>
       </c>
@@ -10315,32 +10286,32 @@
     </row>
     <row r="38" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="62"/>
+      <c r="C38" s="55"/>
       <c r="D38" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="22">
         <v>2</v>
       </c>
-      <c r="F38" s="80">
+      <c r="F38" s="95">
         <v>1.5</v>
       </c>
-      <c r="G38" s="62"/>
-      <c r="H38" s="24">
+      <c r="G38" s="55"/>
+      <c r="H38" s="22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I38" s="1"/>
-      <c r="J38" s="60" t="s">
+      <c r="J38" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="K38" s="62"/>
-      <c r="L38" s="23">
+      <c r="K38" s="55"/>
+      <c r="L38" s="38">
         <f>H32</f>
-        <v>8200</v>
+        <v>5637.5</v>
       </c>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -10359,29 +10330,29 @@
     </row>
     <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="60" t="s">
+      <c r="B39" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="62"/>
+      <c r="C39" s="55"/>
       <c r="D39" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="22">
         <v>2</v>
       </c>
-      <c r="F39" s="80">
+      <c r="F39" s="95">
         <v>2</v>
       </c>
-      <c r="G39" s="62"/>
-      <c r="H39" s="24">
+      <c r="G39" s="55"/>
+      <c r="H39" s="22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I39" s="1"/>
-      <c r="J39" s="60" t="s">
+      <c r="J39" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="K39" s="62"/>
+      <c r="K39" s="55"/>
       <c r="L39" s="12">
         <f>H43</f>
         <v>116</v>
@@ -10403,32 +10374,32 @@
     </row>
     <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="62"/>
+      <c r="C40" s="55"/>
       <c r="D40" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E40" s="22">
         <v>2</v>
       </c>
-      <c r="F40" s="80">
+      <c r="F40" s="95">
         <v>1</v>
       </c>
-      <c r="G40" s="62"/>
-      <c r="H40" s="24">
+      <c r="G40" s="55"/>
+      <c r="H40" s="22">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I40" s="1"/>
-      <c r="J40" s="60" t="s">
+      <c r="J40" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="62"/>
-      <c r="L40" s="30">
+      <c r="K40" s="55"/>
+      <c r="L40" s="28">
         <f>J50</f>
-        <v>739.42836799999998</v>
+        <v>403.85700299999996</v>
       </c>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -10447,32 +10418,32 @@
     </row>
     <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="62"/>
+      <c r="C41" s="55"/>
       <c r="D41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="22">
         <v>2</v>
       </c>
-      <c r="F41" s="80">
+      <c r="F41" s="95">
         <v>1.5</v>
       </c>
-      <c r="G41" s="62"/>
-      <c r="H41" s="24">
+      <c r="G41" s="55"/>
+      <c r="H41" s="22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I41" s="1"/>
-      <c r="J41" s="60" t="s">
+      <c r="J41" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="K41" s="62"/>
-      <c r="L41" s="25">
+      <c r="K41" s="55"/>
+      <c r="L41" s="115">
         <f>L38+L39+L40</f>
-        <v>9055.4283680000008</v>
+        <v>6157.3570030000001</v>
       </c>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -10491,21 +10462,21 @@
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="62"/>
+      <c r="C42" s="55"/>
       <c r="D42" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="22">
         <v>2</v>
       </c>
-      <c r="F42" s="80">
+      <c r="F42" s="95">
         <v>42</v>
       </c>
-      <c r="G42" s="62"/>
-      <c r="H42" s="24">
+      <c r="G42" s="55"/>
+      <c r="H42" s="22">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
@@ -10530,15 +10501,15 @@
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="B43" s="82" t="s">
+      <c r="B43" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="62"/>
-      <c r="H43" s="31">
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="29">
         <f>SUM(H36:H42)</f>
         <v>116</v>
       </c>
@@ -10591,10 +10562,10 @@
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="54"/>
+      <c r="C45" s="74"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -10627,18 +10598,18 @@
       <c r="C46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="97" t="s">
+      <c r="D46" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="62"/>
-      <c r="F46" s="97" t="s">
+      <c r="E46" s="55"/>
+      <c r="F46" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="G46" s="62"/>
-      <c r="H46" s="97" t="s">
+      <c r="G46" s="55"/>
+      <c r="H46" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="I46" s="62"/>
+      <c r="I46" s="55"/>
       <c r="J46" s="3" t="s">
         <v>18</v>
       </c>
@@ -10667,21 +10638,21 @@
       <c r="C47" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="96">
+      <c r="D47" s="69">
         <v>18.66</v>
       </c>
-      <c r="E47" s="62"/>
-      <c r="F47" s="88">
-        <v>4</v>
-      </c>
-      <c r="G47" s="62"/>
-      <c r="H47" s="96">
+      <c r="E47" s="111"/>
+      <c r="F47" s="69">
+        <v>2.75</v>
+      </c>
+      <c r="G47" s="113"/>
+      <c r="H47" s="69">
         <v>0.79620000000000002</v>
       </c>
-      <c r="I47" s="62"/>
-      <c r="J47" s="30">
+      <c r="I47" s="111"/>
+      <c r="J47" s="28">
         <f>D47*F47*H47</f>
-        <v>59.428367999999999</v>
+        <v>40.857002999999999</v>
       </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -10708,21 +10679,21 @@
       <c r="C48" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="88">
-        <v>120</v>
-      </c>
-      <c r="E48" s="62"/>
-      <c r="F48" s="88">
-        <v>4</v>
-      </c>
-      <c r="G48" s="62"/>
-      <c r="H48" s="96">
-        <v>70</v>
-      </c>
-      <c r="I48" s="62"/>
+      <c r="D48" s="114">
+        <v>160</v>
+      </c>
+      <c r="E48" s="111"/>
+      <c r="F48" s="69">
+        <v>2.75</v>
+      </c>
+      <c r="G48" s="113"/>
+      <c r="H48" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="I48" s="111"/>
       <c r="J48" s="12">
-        <f>F48*H48</f>
-        <v>280</v>
+        <f>D48*F48*H48</f>
+        <v>88</v>
       </c>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -10749,21 +10720,21 @@
       <c r="C49" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="88">
+      <c r="D49" s="69">
         <v>2</v>
       </c>
-      <c r="E49" s="62"/>
-      <c r="F49" s="88">
-        <v>4</v>
-      </c>
-      <c r="G49" s="62"/>
-      <c r="H49" s="96">
+      <c r="E49" s="111"/>
+      <c r="F49" s="69">
+        <v>2.75</v>
+      </c>
+      <c r="G49" s="113"/>
+      <c r="H49" s="69">
         <v>50</v>
       </c>
-      <c r="I49" s="62"/>
+      <c r="I49" s="113"/>
       <c r="J49" s="12">
         <f>D49*F49*H49</f>
-        <v>400</v>
+        <v>275</v>
       </c>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -10784,19 +10755,19 @@
     </row>
     <row r="50" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="61"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="32">
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="30">
         <f>SUM(J47:J49)</f>
-        <v>739.42836799999998</v>
+        <v>403.85700299999996</v>
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -10846,11 +10817,11 @@
     <row r="52" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="99" t="s">
+      <c r="C52" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -10876,10 +10847,10 @@
     <row r="53" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="100" t="s">
+      <c r="C53" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="62"/>
+      <c r="D53" s="55"/>
       <c r="E53" s="11" t="s">
         <v>40</v>
       </c>
@@ -10908,11 +10879,11 @@
     <row r="54" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="60" t="s">
+      <c r="C54" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="D54" s="62"/>
-      <c r="E54" s="23">
+      <c r="D54" s="55"/>
+      <c r="E54" s="21">
         <f>M17</f>
         <v>8720</v>
       </c>
@@ -10941,13 +10912,13 @@
     <row r="55" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="60" t="s">
+      <c r="C55" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="62"/>
-      <c r="E55" s="23">
+      <c r="D55" s="55"/>
+      <c r="E55" s="21">
         <f>L41</f>
-        <v>9055.4283680000008</v>
+        <v>6157.3570030000001</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -10974,13 +10945,13 @@
     <row r="56" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="60" t="s">
+      <c r="C56" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="62"/>
-      <c r="E56" s="25">
+      <c r="D56" s="55"/>
+      <c r="E56" s="23">
         <f>E54+E55</f>
-        <v>17775.428368000001</v>
+        <v>14877.357003000001</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -11034,10 +11005,10 @@
     </row>
     <row r="58" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
-      <c r="B58" s="74" t="s">
+      <c r="B58" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="75"/>
+      <c r="C58" s="68"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -11064,11 +11035,11 @@
     </row>
     <row r="59" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
-      <c r="B59" s="70" t="s">
+      <c r="B59" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -11094,16 +11065,16 @@
     </row>
     <row r="60" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
-      <c r="B60" s="84" t="s">
+      <c r="B60" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="62"/>
-      <c r="E60" s="43" t="s">
+      <c r="C60" s="54"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F60" s="44" t="s">
-        <v>64</v>
+      <c r="F60" s="41" t="s">
+        <v>128</v>
       </c>
       <c r="G60" s="11" t="s">
         <v>40</v>
@@ -11129,18 +11100,18 @@
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="101" t="s">
-        <v>65</v>
-      </c>
-      <c r="C61" s="101"/>
-      <c r="D61" s="101"/>
-      <c r="E61" s="42">
+      <c r="B61" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="84"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="39">
         <v>300</v>
       </c>
-      <c r="F61" s="42">
+      <c r="F61" s="110">
         <v>4</v>
       </c>
-      <c r="G61" s="42">
+      <c r="G61" s="39">
         <f>E61*F61</f>
         <v>1200</v>
       </c>
@@ -11165,14 +11136,14 @@
     </row>
     <row r="62" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="82" t="s">
+      <c r="B62" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="62"/>
-      <c r="G62" s="26">
+      <c r="C62" s="54"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="54"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="24">
         <f>G61</f>
         <v>1200</v>
       </c>
@@ -11225,11 +11196,11 @@
     </row>
     <row r="64" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
-      <c r="B64" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
+      <c r="B64" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -11255,30 +11226,30 @@
     </row>
     <row r="65" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
-      <c r="B65" s="84" t="s">
+      <c r="B65" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="62"/>
+      <c r="C65" s="55"/>
       <c r="D65" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="84" t="s">
+      <c r="E65" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="F65" s="55"/>
+      <c r="G65" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="F65" s="62"/>
-      <c r="G65" s="94" t="s">
-        <v>68</v>
-      </c>
-      <c r="H65" s="62"/>
+      <c r="H65" s="55"/>
       <c r="I65" s="11" t="s">
         <v>40</v>
       </c>
       <c r="J65" s="1"/>
-      <c r="K65" s="102" t="s">
-        <v>69</v>
-      </c>
-      <c r="L65" s="47"/>
-      <c r="M65" s="47"/>
+      <c r="K65" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="L65" s="61"/>
+      <c r="M65" s="61"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
@@ -11295,31 +11266,31 @@
     </row>
     <row r="66" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
-      <c r="B66" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="62"/>
+      <c r="B66" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="55"/>
       <c r="D66" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E66" s="82">
+      <c r="E66" s="69">
         <v>1</v>
       </c>
-      <c r="F66" s="62"/>
-      <c r="G66" s="82">
+      <c r="F66" s="55"/>
+      <c r="G66" s="69">
         <v>16</v>
       </c>
-      <c r="H66" s="62"/>
+      <c r="H66" s="55"/>
       <c r="I66" s="12">
         <f t="shared" ref="I66:I68" si="1">G66*E66</f>
         <v>16</v>
       </c>
       <c r="J66" s="1"/>
-      <c r="K66" s="97" t="s">
+      <c r="K66" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="L66" s="61"/>
-      <c r="M66" s="62"/>
+      <c r="L66" s="54"/>
+      <c r="M66" s="55"/>
       <c r="N66" s="13" t="s">
         <v>40</v>
       </c>
@@ -11338,31 +11309,31 @@
     </row>
     <row r="67" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
-      <c r="B67" s="60" t="s">
+      <c r="B67" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="C67" s="62"/>
+      <c r="C67" s="55"/>
       <c r="D67" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E67" s="82">
+      <c r="E67" s="69">
         <v>2</v>
       </c>
-      <c r="F67" s="62"/>
-      <c r="G67" s="82">
+      <c r="F67" s="55"/>
+      <c r="G67" s="69">
         <v>42</v>
       </c>
-      <c r="H67" s="62"/>
+      <c r="H67" s="55"/>
       <c r="I67" s="12">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="J67" s="1"/>
-      <c r="K67" s="103" t="s">
+      <c r="K67" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="L67" s="61"/>
-      <c r="M67" s="62"/>
+      <c r="L67" s="54"/>
+      <c r="M67" s="55"/>
       <c r="N67" s="12">
         <f>G62</f>
         <v>1200</v>
@@ -11382,31 +11353,31 @@
     </row>
     <row r="68" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
-      <c r="B68" s="60" t="s">
+      <c r="B68" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="55"/>
+      <c r="D68" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="62"/>
-      <c r="D68" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E68" s="82">
+      <c r="E68" s="69">
         <v>1</v>
       </c>
-      <c r="F68" s="62"/>
-      <c r="G68" s="82">
+      <c r="F68" s="55"/>
+      <c r="G68" s="69">
         <v>16</v>
       </c>
-      <c r="H68" s="62"/>
+      <c r="H68" s="55"/>
       <c r="I68" s="12">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J68" s="1"/>
-      <c r="K68" s="103" t="s">
-        <v>66</v>
-      </c>
-      <c r="L68" s="61"/>
-      <c r="M68" s="62"/>
+      <c r="K68" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="L68" s="54"/>
+      <c r="M68" s="55"/>
       <c r="N68" s="12">
         <f>I69</f>
         <v>116</v>
@@ -11426,28 +11397,28 @@
     </row>
     <row r="69" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
-      <c r="B69" s="82" t="s">
+      <c r="B69" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C69" s="61"/>
-      <c r="D69" s="61"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="61"/>
-      <c r="G69" s="61"/>
-      <c r="H69" s="62"/>
-      <c r="I69" s="26">
+      <c r="C69" s="54"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="55"/>
+      <c r="I69" s="24">
         <f>SUM(I66:I68)</f>
         <v>116</v>
       </c>
       <c r="J69" s="1"/>
-      <c r="K69" s="103" t="s">
-        <v>73</v>
-      </c>
-      <c r="L69" s="61"/>
-      <c r="M69" s="62"/>
-      <c r="N69" s="33">
+      <c r="K69" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="L69" s="54"/>
+      <c r="M69" s="55"/>
+      <c r="N69" s="31">
         <f>J74</f>
-        <v>59.428367999999999</v>
+        <v>178.28510400000002</v>
       </c>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
@@ -11473,14 +11444,14 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
-      <c r="K70" s="103" t="s">
-        <v>74</v>
-      </c>
-      <c r="L70" s="61"/>
-      <c r="M70" s="62"/>
-      <c r="N70" s="30">
+      <c r="K70" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="L70" s="54"/>
+      <c r="M70" s="55"/>
+      <c r="N70" s="28">
         <f>H84</f>
-        <v>2180</v>
+        <v>1744</v>
       </c>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -11497,25 +11468,25 @@
     </row>
     <row r="71" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
-      <c r="B71" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
+      <c r="B71" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71" s="61"/>
+      <c r="D71" s="61"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
-      <c r="K71" s="82" t="s">
+      <c r="K71" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="L71" s="61"/>
-      <c r="M71" s="62"/>
-      <c r="N71" s="34">
+      <c r="L71" s="54"/>
+      <c r="M71" s="55"/>
+      <c r="N71" s="32">
         <f>N67+N68+N69+N70</f>
-        <v>3555.4283679999999</v>
+        <v>3238.285104</v>
       </c>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -11538,18 +11509,18 @@
       <c r="C72" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D72" s="94" t="s">
+      <c r="D72" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="E72" s="62"/>
-      <c r="F72" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="G72" s="62"/>
-      <c r="H72" s="94" t="s">
+      <c r="E72" s="55"/>
+      <c r="F72" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="G72" s="55"/>
+      <c r="H72" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="I72" s="62"/>
+      <c r="I72" s="55"/>
       <c r="J72" s="13" t="s">
         <v>18</v>
       </c>
@@ -11573,26 +11544,26 @@
     <row r="73" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D73" s="96">
+      <c r="D73" s="69">
         <v>18.66</v>
       </c>
-      <c r="E73" s="62"/>
-      <c r="F73" s="96">
-        <v>4</v>
-      </c>
-      <c r="G73" s="62"/>
-      <c r="H73" s="96">
+      <c r="E73" s="111"/>
+      <c r="F73" s="79">
+        <v>12</v>
+      </c>
+      <c r="G73" s="55"/>
+      <c r="H73" s="79">
         <v>0.79620000000000002</v>
       </c>
-      <c r="I73" s="62"/>
-      <c r="J73" s="33">
+      <c r="I73" s="55"/>
+      <c r="J73" s="31">
         <f>PRODUCT(D73:I73)</f>
-        <v>59.428367999999999</v>
+        <v>178.28510400000002</v>
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -11613,19 +11584,19 @@
     </row>
     <row r="74" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
-      <c r="B74" s="82" t="s">
+      <c r="B74" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C74" s="61"/>
-      <c r="D74" s="61"/>
-      <c r="E74" s="61"/>
-      <c r="F74" s="61"/>
-      <c r="G74" s="61"/>
-      <c r="H74" s="61"/>
-      <c r="I74" s="62"/>
-      <c r="J74" s="35">
+      <c r="C74" s="54"/>
+      <c r="D74" s="54"/>
+      <c r="E74" s="54"/>
+      <c r="F74" s="54"/>
+      <c r="G74" s="54"/>
+      <c r="H74" s="54"/>
+      <c r="I74" s="55"/>
+      <c r="J74" s="33">
         <f>J73</f>
-        <v>59.428367999999999</v>
+        <v>178.28510400000002</v>
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -11675,7 +11646,7 @@
     <row r="76" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -11704,11 +11675,11 @@
     </row>
     <row r="77" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
-      <c r="B77" s="83" t="s">
+      <c r="B77" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="C77" s="61"/>
-      <c r="D77" s="62"/>
+      <c r="C77" s="54"/>
+      <c r="D77" s="55"/>
       <c r="E77" s="3" t="s">
         <v>5</v>
       </c>
@@ -11716,17 +11687,16 @@
         <v>6</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H77" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I77" s="15"/>
+      <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
@@ -11742,31 +11712,30 @@
     </row>
     <row r="78" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
-      <c r="B78" s="50" t="s">
+      <c r="B78" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C78" s="51"/>
-      <c r="D78" s="52"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="72"/>
       <c r="E78" s="56">
         <v>1</v>
       </c>
-      <c r="F78" s="57">
+      <c r="F78" s="58">
         <f>G7</f>
         <v>4200</v>
       </c>
-      <c r="G78" s="58">
-        <v>0.25</v>
-      </c>
-      <c r="H78" s="48">
-        <f>(E78*F78)*G78</f>
-        <v>1050</v>
-      </c>
-      <c r="I78" s="46"/>
+      <c r="G78" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="H78" s="60">
+        <f>(F78)*G78*E78</f>
+        <v>840</v>
+      </c>
+      <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
@@ -11782,19 +11751,18 @@
     </row>
     <row r="79" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
-      <c r="B79" s="53"/>
-      <c r="C79" s="54"/>
-      <c r="D79" s="55"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="47"/>
+      <c r="B79" s="73"/>
+      <c r="C79" s="74"/>
+      <c r="D79" s="75"/>
+      <c r="E79" s="57"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="57"/>
+      <c r="H79" s="57"/>
+      <c r="I79" s="112"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
@@ -11810,31 +11778,30 @@
     </row>
     <row r="80" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
-      <c r="B80" s="50" t="s">
+      <c r="B80" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="51"/>
-      <c r="D80" s="52"/>
+      <c r="C80" s="71"/>
+      <c r="D80" s="72"/>
       <c r="E80" s="56">
         <v>1</v>
       </c>
-      <c r="F80" s="57">
+      <c r="F80" s="58">
         <f>G9</f>
         <v>3800</v>
       </c>
-      <c r="G80" s="58">
-        <v>0.25</v>
-      </c>
-      <c r="H80" s="48">
-        <f>(E80*F80)*G80</f>
-        <v>950</v>
-      </c>
-      <c r="I80" s="46"/>
+      <c r="G80" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="H80" s="60">
+        <f t="shared" ref="H80" si="2">(F80)*G80*E80</f>
+        <v>760</v>
+      </c>
+      <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
@@ -11850,19 +11817,18 @@
     </row>
     <row r="81" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
-      <c r="B81" s="53"/>
-      <c r="C81" s="54"/>
-      <c r="D81" s="55"/>
-      <c r="E81" s="49"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="59"/>
-      <c r="H81" s="49"/>
-      <c r="I81" s="47"/>
+      <c r="B81" s="73"/>
+      <c r="C81" s="74"/>
+      <c r="D81" s="75"/>
+      <c r="E81" s="57"/>
+      <c r="F81" s="57"/>
+      <c r="G81" s="57"/>
+      <c r="H81" s="57"/>
+      <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
@@ -11878,30 +11844,29 @@
     </row>
     <row r="82" spans="1:26" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
-      <c r="B82" s="50" t="s">
+      <c r="B82" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C82" s="51"/>
-      <c r="D82" s="52"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="72"/>
       <c r="E82" s="56">
         <v>1</v>
       </c>
-      <c r="F82" s="57">
+      <c r="F82" s="58">
         <v>720</v>
       </c>
-      <c r="G82" s="58">
-        <v>0.25</v>
-      </c>
-      <c r="H82" s="48">
-        <f>(E82*F82)*G82</f>
-        <v>180</v>
-      </c>
-      <c r="I82" s="46"/>
+      <c r="G82" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="H82" s="60">
+        <f t="shared" ref="H82" si="3">(F82)*G82*E82</f>
+        <v>144</v>
+      </c>
+      <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
@@ -11917,19 +11882,18 @@
     </row>
     <row r="83" spans="1:26" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
-      <c r="B83" s="53"/>
-      <c r="C83" s="54"/>
-      <c r="D83" s="55"/>
-      <c r="E83" s="49"/>
-      <c r="F83" s="49"/>
-      <c r="G83" s="59"/>
-      <c r="H83" s="49"/>
-      <c r="I83" s="47"/>
+      <c r="B83" s="73"/>
+      <c r="C83" s="74"/>
+      <c r="D83" s="75"/>
+      <c r="E83" s="57"/>
+      <c r="F83" s="57"/>
+      <c r="G83" s="57"/>
+      <c r="H83" s="57"/>
+      <c r="I83" s="1"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
@@ -11945,24 +11909,23 @@
     </row>
     <row r="84" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
-      <c r="B84" s="82" t="s">
+      <c r="B84" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C84" s="61"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="61"/>
-      <c r="F84" s="61"/>
-      <c r="G84" s="61"/>
-      <c r="H84" s="35">
+      <c r="C84" s="54"/>
+      <c r="D84" s="54"/>
+      <c r="E84" s="54"/>
+      <c r="F84" s="54"/>
+      <c r="G84" s="54"/>
+      <c r="H84" s="33">
         <f>SUM(H78:H82)</f>
-        <v>2180</v>
-      </c>
-      <c r="I84" s="36"/>
+        <v>1744</v>
+      </c>
+      <c r="I84" s="1"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
-      <c r="N84" s="1"/>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
@@ -11990,7 +11953,6 @@
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
-      <c r="N85" s="1"/>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
@@ -12006,10 +11968,10 @@
     </row>
     <row r="86" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
-      <c r="B86" s="74" t="s">
-        <v>78</v>
-      </c>
-      <c r="C86" s="75"/>
+      <c r="B86" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C86" s="68"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -12020,7 +11982,6 @@
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
-      <c r="N86" s="1"/>
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
@@ -12036,10 +11997,10 @@
     </row>
     <row r="87" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
-      <c r="B87" s="70" t="s">
-        <v>79</v>
-      </c>
-      <c r="C87" s="47"/>
+      <c r="B87" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="61"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -12066,18 +12027,18 @@
     </row>
     <row r="88" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
-      <c r="B88" s="97" t="s">
+      <c r="B88" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C88" s="62"/>
-      <c r="D88" s="83" t="s">
-        <v>80</v>
-      </c>
-      <c r="E88" s="62"/>
-      <c r="F88" s="16" t="s">
+      <c r="C88" s="55"/>
+      <c r="D88" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="E88" s="55"/>
+      <c r="F88" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G88" s="17" t="s">
+      <c r="G88" s="16" t="s">
         <v>18</v>
       </c>
       <c r="H88" s="1"/>
@@ -12102,18 +12063,18 @@
     </row>
     <row r="89" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
-      <c r="B89" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="C89" s="62"/>
-      <c r="D89" s="63">
+      <c r="B89" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C89" s="55"/>
+      <c r="D89" s="65">
         <v>1025</v>
       </c>
-      <c r="E89" s="62"/>
-      <c r="F89" s="37">
+      <c r="E89" s="55"/>
+      <c r="F89" s="34">
         <v>12</v>
       </c>
-      <c r="G89" s="38">
+      <c r="G89" s="35">
         <f>D89*F89</f>
         <v>12300</v>
       </c>
@@ -12139,19 +12100,19 @@
     </row>
     <row r="90" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
-      <c r="B90" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" s="62"/>
-      <c r="D90" s="63">
+      <c r="B90" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C90" s="55"/>
+      <c r="D90" s="65">
         <v>500</v>
       </c>
-      <c r="E90" s="62"/>
-      <c r="F90" s="37">
+      <c r="E90" s="55"/>
+      <c r="F90" s="34">
         <v>12</v>
       </c>
-      <c r="G90" s="38">
-        <f t="shared" ref="G90:G91" si="2">D90*F90</f>
+      <c r="G90" s="35">
+        <f>D90*F90</f>
         <v>6000</v>
       </c>
       <c r="H90" s="1"/>
@@ -12176,19 +12137,19 @@
     </row>
     <row r="91" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
-      <c r="B91" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="C91" s="62"/>
-      <c r="D91" s="63">
+      <c r="B91" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C91" s="55"/>
+      <c r="D91" s="65">
         <v>30</v>
       </c>
-      <c r="E91" s="62"/>
-      <c r="F91" s="37">
+      <c r="E91" s="55"/>
+      <c r="F91" s="34">
         <v>12</v>
       </c>
-      <c r="G91" s="38">
-        <f t="shared" si="2"/>
+      <c r="G91" s="35">
+        <f>D91*F91</f>
         <v>360</v>
       </c>
       <c r="H91" s="1"/>
@@ -12213,14 +12174,14 @@
     </row>
     <row r="92" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
-      <c r="B92" s="60" t="s">
+      <c r="B92" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="C92" s="61"/>
-      <c r="D92" s="61"/>
-      <c r="E92" s="61"/>
-      <c r="F92" s="62"/>
-      <c r="G92" s="39">
+      <c r="C92" s="54"/>
+      <c r="D92" s="54"/>
+      <c r="E92" s="54"/>
+      <c r="F92" s="55"/>
+      <c r="G92" s="36">
         <f>SUM(G89:G91)</f>
         <v>18660</v>
       </c>
@@ -12246,9 +12207,9 @@
     </row>
     <row r="93" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
@@ -12274,11 +12235,11 @@
     </row>
     <row r="94" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
-      <c r="B94" s="104" t="s">
-        <v>84</v>
-      </c>
-      <c r="C94" s="47"/>
-      <c r="D94" s="47"/>
+      <c r="B94" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
@@ -12304,14 +12265,14 @@
     </row>
     <row r="95" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
-      <c r="B95" s="97" t="s">
+      <c r="B95" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C95" s="55"/>
+      <c r="D95" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="C95" s="62"/>
-      <c r="D95" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="E95" s="62"/>
+      <c r="E95" s="55"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -12336,15 +12297,15 @@
     </row>
     <row r="96" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
-      <c r="B96" s="60" t="s">
-        <v>87</v>
-      </c>
-      <c r="C96" s="62"/>
-      <c r="D96" s="64">
+      <c r="B96" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C96" s="55"/>
+      <c r="D96" s="106">
         <f>G92</f>
         <v>18660</v>
       </c>
-      <c r="E96" s="62"/>
+      <c r="E96" s="55"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -12369,15 +12330,15 @@
     </row>
     <row r="97" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
-      <c r="B97" s="60" t="s">
+      <c r="B97" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="C97" s="62"/>
-      <c r="D97" s="65">
+      <c r="C97" s="55"/>
+      <c r="D97" s="107">
         <f>D96</f>
         <v>18660</v>
       </c>
-      <c r="E97" s="62"/>
+      <c r="E97" s="55"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
@@ -12431,7 +12392,7 @@
     <row r="99" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -12460,22 +12421,22 @@
     </row>
     <row r="100" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
-      <c r="B100" s="66" t="s">
+      <c r="B100" s="108" t="s">
+        <v>87</v>
+      </c>
+      <c r="C100" s="54"/>
+      <c r="D100" s="55"/>
+      <c r="E100" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C100" s="61"/>
-      <c r="D100" s="62"/>
-      <c r="E100" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="H100" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -12498,21 +12459,21 @@
     </row>
     <row r="101" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
-      <c r="B101" s="67" t="s">
-        <v>94</v>
-      </c>
-      <c r="C101" s="61"/>
-      <c r="D101" s="62"/>
-      <c r="E101" s="40">
+      <c r="B101" s="109" t="s">
+        <v>92</v>
+      </c>
+      <c r="C101" s="54"/>
+      <c r="D101" s="55"/>
+      <c r="E101" s="37">
         <v>2024</v>
       </c>
-      <c r="F101" s="40">
+      <c r="F101" s="37">
         <v>2025</v>
       </c>
-      <c r="G101" s="40">
+      <c r="G101" s="37">
         <v>2026</v>
       </c>
-      <c r="H101" s="40">
+      <c r="H101" s="37">
         <v>2027</v>
       </c>
       <c r="I101" s="1"/>
@@ -12536,22 +12497,22 @@
     </row>
     <row r="102" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
-      <c r="B102" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="C102" s="61"/>
-      <c r="D102" s="62"/>
-      <c r="E102" s="41"/>
-      <c r="F102" s="41">
-        <f t="shared" ref="F102:H102" si="3">$D$97</f>
+      <c r="B102" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="C102" s="54"/>
+      <c r="D102" s="55"/>
+      <c r="E102" s="38"/>
+      <c r="F102" s="38">
+        <f t="shared" ref="F102:H102" si="4">$D$97</f>
         <v>18660</v>
       </c>
-      <c r="G102" s="41">
-        <f t="shared" si="3"/>
+      <c r="G102" s="38">
+        <f t="shared" si="4"/>
         <v>18660</v>
       </c>
-      <c r="H102" s="41">
-        <f t="shared" si="3"/>
+      <c r="H102" s="38">
+        <f t="shared" si="4"/>
         <v>18660</v>
       </c>
       <c r="I102" s="1"/>
@@ -12575,22 +12536,22 @@
     </row>
     <row r="103" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
-      <c r="B103" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="C103" s="61"/>
-      <c r="D103" s="62"/>
-      <c r="E103" s="41"/>
-      <c r="F103" s="41">
+      <c r="B103" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" s="54"/>
+      <c r="D103" s="55"/>
+      <c r="E103" s="38"/>
+      <c r="F103" s="38">
         <f>$D$97</f>
         <v>18660</v>
       </c>
-      <c r="G103" s="41">
-        <f t="shared" ref="G103:H103" si="4">$D$97</f>
+      <c r="G103" s="38">
+        <f t="shared" ref="G103:H103" si="5">$D$97</f>
         <v>18660</v>
       </c>
-      <c r="H103" s="41">
-        <f t="shared" si="4"/>
+      <c r="H103" s="38">
+        <f t="shared" si="5"/>
         <v>18660</v>
       </c>
       <c r="I103" s="1"/>
@@ -12614,15 +12575,15 @@
     </row>
     <row r="104" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
-      <c r="B104" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C104" s="61"/>
-      <c r="D104" s="62"/>
-      <c r="E104" s="41"/>
-      <c r="F104" s="41"/>
-      <c r="G104" s="41"/>
-      <c r="H104" s="41"/>
+      <c r="B104" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C104" s="54"/>
+      <c r="D104" s="55"/>
+      <c r="E104" s="38"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="38"/>
+      <c r="H104" s="38"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
@@ -12644,23 +12605,23 @@
     </row>
     <row r="105" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
-      <c r="B105" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="C105" s="61"/>
-      <c r="D105" s="62"/>
-      <c r="E105" s="41"/>
-      <c r="F105" s="41">
+      <c r="B105" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C105" s="54"/>
+      <c r="D105" s="55"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38">
         <f>N71</f>
-        <v>3555.4283679999999</v>
-      </c>
-      <c r="G105" s="41">
+        <v>3238.285104</v>
+      </c>
+      <c r="G105" s="38">
         <f>N71</f>
-        <v>3555.4283679999999</v>
-      </c>
-      <c r="H105" s="41">
+        <v>3238.285104</v>
+      </c>
+      <c r="H105" s="38">
         <f>N71</f>
-        <v>3555.4283679999999</v>
+        <v>3238.285104</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
@@ -12683,23 +12644,23 @@
     </row>
     <row r="106" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
-      <c r="B106" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="C106" s="61"/>
-      <c r="D106" s="62"/>
-      <c r="E106" s="41"/>
-      <c r="F106" s="41">
+      <c r="B106" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C106" s="54"/>
+      <c r="D106" s="55"/>
+      <c r="E106" s="38"/>
+      <c r="F106" s="38">
         <f>F105</f>
-        <v>3555.4283679999999</v>
-      </c>
-      <c r="G106" s="41">
-        <f t="shared" ref="G106:H106" si="5">G105</f>
-        <v>3555.4283679999999</v>
-      </c>
-      <c r="H106" s="41">
-        <f t="shared" si="5"/>
-        <v>3555.4283679999999</v>
+        <v>3238.285104</v>
+      </c>
+      <c r="G106" s="38">
+        <f t="shared" ref="G106:H106" si="6">G105</f>
+        <v>3238.285104</v>
+      </c>
+      <c r="H106" s="38">
+        <f t="shared" si="6"/>
+        <v>3238.285104</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
@@ -12722,15 +12683,15 @@
     </row>
     <row r="107" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
-      <c r="B107" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="C107" s="61"/>
-      <c r="D107" s="62"/>
-      <c r="E107" s="41"/>
-      <c r="F107" s="41"/>
-      <c r="G107" s="41"/>
-      <c r="H107" s="41"/>
+      <c r="B107" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C107" s="54"/>
+      <c r="D107" s="55"/>
+      <c r="E107" s="38"/>
+      <c r="F107" s="38"/>
+      <c r="G107" s="38"/>
+      <c r="H107" s="38"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
@@ -12752,23 +12713,23 @@
     </row>
     <row r="108" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
-      <c r="B108" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="C108" s="61"/>
-      <c r="D108" s="62"/>
-      <c r="E108" s="41"/>
-      <c r="F108" s="41">
+      <c r="B108" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C108" s="54"/>
+      <c r="D108" s="55"/>
+      <c r="E108" s="38"/>
+      <c r="F108" s="38">
         <f>F103-F106</f>
-        <v>15104.571631999999</v>
-      </c>
-      <c r="G108" s="41">
+        <v>15421.714895999999</v>
+      </c>
+      <c r="G108" s="38">
         <f>G103-G106</f>
-        <v>15104.571631999999</v>
-      </c>
-      <c r="H108" s="41">
+        <v>15421.714895999999</v>
+      </c>
+      <c r="H108" s="38">
         <f>H103-H106</f>
-        <v>15104.571631999999</v>
+        <v>15421.714895999999</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
@@ -12791,15 +12752,15 @@
     </row>
     <row r="109" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
-      <c r="B109" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="C109" s="61"/>
-      <c r="D109" s="62"/>
-      <c r="E109" s="41"/>
-      <c r="F109" s="41"/>
-      <c r="G109" s="41"/>
-      <c r="H109" s="41"/>
+      <c r="B109" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C109" s="54"/>
+      <c r="D109" s="55"/>
+      <c r="E109" s="38"/>
+      <c r="F109" s="38"/>
+      <c r="G109" s="38"/>
+      <c r="H109" s="38"/>
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
@@ -12821,15 +12782,15 @@
     </row>
     <row r="110" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
-      <c r="B110" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="C110" s="61"/>
-      <c r="D110" s="62"/>
-      <c r="E110" s="41"/>
-      <c r="F110" s="41"/>
-      <c r="G110" s="41"/>
-      <c r="H110" s="41"/>
+      <c r="B110" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="C110" s="54"/>
+      <c r="D110" s="55"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
+      <c r="G110" s="38"/>
+      <c r="H110" s="38"/>
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
@@ -12851,18 +12812,18 @@
     </row>
     <row r="111" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
-      <c r="B111" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="C111" s="61"/>
-      <c r="D111" s="62"/>
-      <c r="E111" s="41">
+      <c r="B111" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C111" s="54"/>
+      <c r="D111" s="55"/>
+      <c r="E111" s="38">
         <f>I13</f>
         <v>8720</v>
       </c>
-      <c r="F111" s="41"/>
-      <c r="G111" s="41"/>
-      <c r="H111" s="41"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="38"/>
+      <c r="H111" s="38"/>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
@@ -12884,17 +12845,17 @@
     </row>
     <row r="112" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
-      <c r="B112" s="60" t="s">
-        <v>105</v>
-      </c>
-      <c r="C112" s="61"/>
-      <c r="D112" s="62"/>
-      <c r="E112" s="41">
+      <c r="B112" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C112" s="54"/>
+      <c r="D112" s="55"/>
+      <c r="E112" s="38">
         <v>0</v>
       </c>
-      <c r="F112" s="41"/>
-      <c r="G112" s="41"/>
-      <c r="H112" s="41"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -12916,17 +12877,17 @@
     </row>
     <row r="113" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
-      <c r="B113" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="C113" s="61"/>
-      <c r="D113" s="62"/>
-      <c r="E113" s="41">
+      <c r="B113" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="C113" s="54"/>
+      <c r="D113" s="55"/>
+      <c r="E113" s="38">
         <v>0</v>
       </c>
-      <c r="F113" s="41"/>
-      <c r="G113" s="41"/>
-      <c r="H113" s="41"/>
+      <c r="F113" s="38"/>
+      <c r="G113" s="38"/>
+      <c r="H113" s="38"/>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -12948,15 +12909,15 @@
     </row>
     <row r="114" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
-      <c r="B114" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="C114" s="61"/>
-      <c r="D114" s="62"/>
-      <c r="E114" s="41"/>
-      <c r="F114" s="41"/>
-      <c r="G114" s="41"/>
-      <c r="H114" s="41"/>
+      <c r="B114" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C114" s="54"/>
+      <c r="D114" s="55"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
+      <c r="G114" s="38"/>
+      <c r="H114" s="38"/>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
@@ -12978,18 +12939,18 @@
     </row>
     <row r="115" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
-      <c r="B115" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="C115" s="61"/>
-      <c r="D115" s="62"/>
-      <c r="E115" s="41">
+      <c r="B115" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="C115" s="54"/>
+      <c r="D115" s="55"/>
+      <c r="E115" s="38">
         <f>H32</f>
-        <v>8200</v>
-      </c>
-      <c r="F115" s="41"/>
-      <c r="G115" s="41"/>
-      <c r="H115" s="41"/>
+        <v>5637.5</v>
+      </c>
+      <c r="F115" s="38"/>
+      <c r="G115" s="38"/>
+      <c r="H115" s="38"/>
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
@@ -13011,18 +12972,18 @@
     </row>
     <row r="116" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
-      <c r="B116" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="C116" s="61"/>
-      <c r="D116" s="62"/>
-      <c r="E116" s="41">
+      <c r="B116" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C116" s="54"/>
+      <c r="D116" s="55"/>
+      <c r="E116" s="38">
         <f>H43</f>
         <v>116</v>
       </c>
-      <c r="F116" s="41"/>
-      <c r="G116" s="41"/>
-      <c r="H116" s="41"/>
+      <c r="F116" s="38"/>
+      <c r="G116" s="38"/>
+      <c r="H116" s="38"/>
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -13044,18 +13005,18 @@
     </row>
     <row r="117" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
-      <c r="B117" s="60" t="s">
+      <c r="B117" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C117" s="61"/>
-      <c r="D117" s="62"/>
-      <c r="E117" s="41">
+      <c r="C117" s="54"/>
+      <c r="D117" s="55"/>
+      <c r="E117" s="38">
         <f>J50</f>
-        <v>739.42836799999998</v>
-      </c>
-      <c r="F117" s="41"/>
-      <c r="G117" s="41"/>
-      <c r="H117" s="41"/>
+        <v>403.85700299999996</v>
+      </c>
+      <c r="F117" s="38"/>
+      <c r="G117" s="38"/>
+      <c r="H117" s="38"/>
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
@@ -13077,26 +13038,26 @@
     </row>
     <row r="118" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
-      <c r="B118" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="C118" s="61"/>
-      <c r="D118" s="62"/>
-      <c r="E118" s="117">
+      <c r="B118" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C118" s="54"/>
+      <c r="D118" s="55"/>
+      <c r="E118" s="52">
         <f>SUM(E111:E117)</f>
-        <v>17775.428368000001</v>
-      </c>
-      <c r="F118" s="27">
+        <v>14877.357002999999</v>
+      </c>
+      <c r="F118" s="25">
         <f>F108</f>
-        <v>15104.571631999999</v>
-      </c>
-      <c r="G118" s="27">
-        <f t="shared" ref="G118:H118" si="6">G108</f>
-        <v>15104.571631999999</v>
-      </c>
-      <c r="H118" s="27">
-        <f t="shared" si="6"/>
-        <v>15104.571631999999</v>
+        <v>15421.714895999999</v>
+      </c>
+      <c r="G118" s="25">
+        <f t="shared" ref="G118:H118" si="7">G108</f>
+        <v>15421.714895999999</v>
+      </c>
+      <c r="H118" s="25">
+        <f t="shared" si="7"/>
+        <v>15421.714895999999</v>
       </c>
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
@@ -13175,10 +13136,10 @@
     </row>
     <row r="121" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
-      <c r="B121" s="74" t="s">
-        <v>111</v>
-      </c>
-      <c r="C121" s="75"/>
+      <c r="B121" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="C121" s="68"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -13205,10 +13166,10 @@
     </row>
     <row r="122" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
-      <c r="B122" s="70" t="s">
-        <v>112</v>
-      </c>
-      <c r="C122" s="47"/>
+      <c r="B122" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C122" s="61"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -13235,9 +13196,9 @@
     </row>
     <row r="123" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
-      <c r="B123" s="76"/>
-      <c r="C123" s="47"/>
-      <c r="D123" s="47"/>
+      <c r="B123" s="101"/>
+      <c r="C123" s="61"/>
+      <c r="D123" s="61"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
@@ -13437,14 +13398,14 @@
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
-      <c r="H130" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="I130" s="47"/>
-      <c r="J130" s="47"/>
-      <c r="K130" s="47"/>
-      <c r="L130" s="47"/>
-      <c r="M130" s="47"/>
+      <c r="H130" s="102" t="s">
+        <v>111</v>
+      </c>
+      <c r="I130" s="61"/>
+      <c r="J130" s="61"/>
+      <c r="K130" s="61"/>
+      <c r="L130" s="61"/>
+      <c r="M130" s="61"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
       <c r="P130" s="1"/>
@@ -13582,7 +13543,7 @@
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
       <c r="L135" s="1">
-        <v>8.0299999999999996E-2</v>
+        <v>0.15140000000000001</v>
       </c>
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
@@ -13663,12 +13624,12 @@
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
-      <c r="I138" s="110" t="s">
-        <v>126</v>
-      </c>
-      <c r="J138" s="105">
+      <c r="I138" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="J138" s="43">
         <f>(F108/(1+L135)^1)+(F108/(1+L135)^2)+(F108/(1+L135)^3)</f>
-        <v>38904.884372229586</v>
+        <v>35129.65772909877</v>
       </c>
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
@@ -13778,14 +13739,14 @@
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
-      <c r="H142" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="I142" s="47"/>
-      <c r="J142" s="47"/>
-      <c r="K142" s="47"/>
-      <c r="L142" s="47"/>
-      <c r="M142" s="47"/>
+      <c r="H142" s="104" t="s">
+        <v>111</v>
+      </c>
+      <c r="I142" s="61"/>
+      <c r="J142" s="61"/>
+      <c r="K142" s="61"/>
+      <c r="L142" s="61"/>
+      <c r="M142" s="61"/>
       <c r="N142" s="1"/>
       <c r="O142" s="1"/>
       <c r="P142" s="1"/>
@@ -13998,7 +13959,7 @@
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
-      <c r="H150" s="19"/>
+      <c r="H150" s="18"/>
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
@@ -14083,12 +14044,12 @@
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
-      <c r="I153" s="108" t="s">
-        <v>127</v>
-      </c>
-      <c r="J153" s="107">
+      <c r="I153" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="J153" s="45">
         <f>E118 + (F106/(1+L135)^1) +  (F106/(1+L135)^2) +  (F106/(1+L135)^3)</f>
-        <v>26933.154447284345</v>
+        <v>22253.958639064836</v>
       </c>
       <c r="K153" s="1"/>
       <c r="L153" s="1"/>
@@ -14199,14 +14160,14 @@
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
-      <c r="H157" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="I157" s="47"/>
-      <c r="J157" s="47"/>
-      <c r="K157" s="47"/>
-      <c r="L157" s="47"/>
-      <c r="M157" s="47"/>
+      <c r="H157" s="103" t="s">
+        <v>112</v>
+      </c>
+      <c r="I157" s="61"/>
+      <c r="J157" s="61"/>
+      <c r="K157" s="61"/>
+      <c r="L157" s="61"/>
+      <c r="M157" s="61"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1"/>
       <c r="P157" s="1"/>
@@ -14229,12 +14190,12 @@
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
-      <c r="H158" s="47"/>
-      <c r="I158" s="47"/>
-      <c r="J158" s="47"/>
-      <c r="K158" s="47"/>
-      <c r="L158" s="47"/>
-      <c r="M158" s="47"/>
+      <c r="H158" s="61"/>
+      <c r="I158" s="61"/>
+      <c r="J158" s="61"/>
+      <c r="K158" s="61"/>
+      <c r="L158" s="61"/>
+      <c r="M158" s="61"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1"/>
       <c r="P158" s="1"/>
@@ -14257,12 +14218,12 @@
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
-      <c r="H159" s="47"/>
-      <c r="I159" s="47"/>
-      <c r="J159" s="47"/>
-      <c r="K159" s="47"/>
-      <c r="L159" s="47"/>
-      <c r="M159" s="47"/>
+      <c r="H159" s="61"/>
+      <c r="I159" s="61"/>
+      <c r="J159" s="61"/>
+      <c r="K159" s="61"/>
+      <c r="L159" s="61"/>
+      <c r="M159" s="61"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1"/>
       <c r="P159" s="1"/>
@@ -14447,21 +14408,21 @@
     </row>
     <row r="166" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
-      <c r="B166" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="C166" s="20"/>
+      <c r="B166" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C166" s="19"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
-      <c r="I166" s="108" t="s">
-        <v>129</v>
-      </c>
-      <c r="J166" s="109">
+      <c r="I166" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="J166" s="47">
         <f>J138-J153</f>
-        <v>11971.729924945241</v>
+        <v>12875.699090033933</v>
       </c>
       <c r="K166" s="1"/>
       <c r="L166" s="1"/>
@@ -14516,15 +14477,15 @@
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
-      <c r="H168" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="I168" s="47"/>
-      <c r="J168" s="47"/>
-      <c r="K168" s="47"/>
-      <c r="L168" s="47"/>
-      <c r="M168" s="47"/>
-      <c r="N168" s="47"/>
+      <c r="H168" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="I168" s="61"/>
+      <c r="J168" s="61"/>
+      <c r="K168" s="61"/>
+      <c r="L168" s="61"/>
+      <c r="M168" s="61"/>
+      <c r="N168" s="61"/>
       <c r="O168" s="1"/>
       <c r="P168" s="1"/>
       <c r="Q168" s="1"/>
@@ -14658,10 +14619,10 @@
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
-      <c r="H173" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="I173" s="47"/>
+      <c r="H173" s="97" t="s">
+        <v>115</v>
+      </c>
+      <c r="I173" s="61"/>
       <c r="J173" s="1"/>
       <c r="K173" s="1"/>
       <c r="L173" s="1"/>
@@ -14688,20 +14649,8 @@
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
-      <c r="H174" s="120" t="s">
-        <v>90</v>
-      </c>
-      <c r="I174" s="121" t="s">
-        <v>91</v>
-      </c>
-      <c r="J174" s="121" t="s">
-        <v>92</v>
-      </c>
-      <c r="K174" s="121" t="s">
-        <v>93</v>
-      </c>
       <c r="L174" s="1"/>
-      <c r="M174" s="27"/>
+      <c r="M174" s="25"/>
       <c r="N174" s="1"/>
       <c r="O174" s="1"/>
       <c r="P174" s="1"/>
@@ -14724,18 +14673,6 @@
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
-      <c r="H175" s="122" t="s">
-        <v>118</v>
-      </c>
-      <c r="I175" s="123" t="s">
-        <v>119</v>
-      </c>
-      <c r="J175" s="123" t="s">
-        <v>119</v>
-      </c>
-      <c r="K175" s="123" t="s">
-        <v>119</v>
-      </c>
       <c r="L175" s="1"/>
       <c r="M175" s="1"/>
       <c r="N175" s="1"/>
@@ -14760,24 +14697,8 @@
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
-      <c r="H176" s="118">
-        <f>-(E118)</f>
-        <v>-17775.428368000001</v>
-      </c>
-      <c r="I176" s="119">
-        <f>F118</f>
-        <v>15104.571631999999</v>
-      </c>
-      <c r="J176" s="119">
-        <f>G118</f>
-        <v>15104.571631999999</v>
-      </c>
-      <c r="K176" s="119">
-        <f>H118</f>
-        <v>15104.571631999999</v>
-      </c>
       <c r="L176" s="1"/>
-      <c r="M176" s="45"/>
+      <c r="M176" s="42"/>
       <c r="N176" s="1"/>
       <c r="O176" s="1"/>
       <c r="P176" s="1"/>
@@ -14800,15 +14721,6 @@
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
-      <c r="H177" s="114" t="s">
-        <v>120</v>
-      </c>
-      <c r="I177" s="115"/>
-      <c r="J177" s="116"/>
-      <c r="K177" s="21">
-        <f>IRR(H176:K176)</f>
-        <v>0.66596894238555615</v>
-      </c>
       <c r="L177" s="1"/>
       <c r="M177" s="1"/>
       <c r="N177" s="1"/>
@@ -14863,8 +14775,8 @@
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
-      <c r="J179" s="113"/>
-      <c r="K179" s="112"/>
+      <c r="J179" s="51"/>
+      <c r="K179" s="50"/>
       <c r="L179" s="1"/>
       <c r="M179" s="1"/>
       <c r="N179" s="1"/>
@@ -14946,7 +14858,7 @@
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
-      <c r="J182" s="27"/>
+      <c r="J182" s="25"/>
       <c r="K182" s="1"/>
       <c r="L182" s="1"/>
       <c r="M182" s="1"/>
@@ -14966,10 +14878,10 @@
     </row>
     <row r="183" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1"/>
-      <c r="B183" s="70" t="s">
-        <v>121</v>
-      </c>
-      <c r="C183" s="47"/>
+      <c r="B183" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C183" s="61"/>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
@@ -15165,12 +15077,12 @@
     <row r="190" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
-      <c r="C190" s="111" t="s">
-        <v>128</v>
-      </c>
-      <c r="D190" s="106">
+      <c r="C190" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="D190" s="44">
         <f>J138/J153</f>
-        <v>1.4444978752257644</v>
+        <v>1.5785801662914838</v>
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
@@ -15198,8 +15110,8 @@
     <row r="191" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
-      <c r="C191" s="20"/>
-      <c r="D191" s="20"/>
+      <c r="C191" s="19"/>
+      <c r="D191" s="19"/>
       <c r="E191" s="1"/>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
@@ -15225,11 +15137,11 @@
     </row>
     <row r="192" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
-      <c r="B192" s="71" t="s">
-        <v>122</v>
-      </c>
-      <c r="C192" s="72"/>
-      <c r="D192" s="72"/>
+      <c r="B192" s="98" t="s">
+        <v>120</v>
+      </c>
+      <c r="C192" s="99"/>
+      <c r="D192" s="99"/>
       <c r="E192" s="1"/>
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
@@ -15561,11 +15473,11 @@
     </row>
     <row r="205" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1"/>
-      <c r="B205" s="70" t="s">
-        <v>123</v>
-      </c>
-      <c r="C205" s="47"/>
-      <c r="D205" s="47"/>
+      <c r="B205" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C205" s="61"/>
+      <c r="D205" s="61"/>
       <c r="E205" s="1"/>
       <c r="F205" s="1"/>
       <c r="G205" s="1"/>
@@ -15591,14 +15503,14 @@
     </row>
     <row r="206" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1"/>
-      <c r="B206" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="C206" s="47"/>
-      <c r="D206" s="47"/>
-      <c r="E206" s="47"/>
-      <c r="F206" s="47"/>
-      <c r="G206" s="47"/>
+      <c r="B206" s="100" t="s">
+        <v>122</v>
+      </c>
+      <c r="C206" s="61"/>
+      <c r="D206" s="61"/>
+      <c r="E206" s="61"/>
+      <c r="F206" s="61"/>
+      <c r="G206" s="61"/>
       <c r="H206" s="1"/>
       <c r="I206" s="1"/>
       <c r="J206" s="1"/>
@@ -15621,12 +15533,12 @@
     </row>
     <row r="207" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1"/>
-      <c r="B207" s="47"/>
-      <c r="C207" s="47"/>
-      <c r="D207" s="47"/>
-      <c r="E207" s="47"/>
-      <c r="F207" s="47"/>
-      <c r="G207" s="47"/>
+      <c r="B207" s="61"/>
+      <c r="C207" s="61"/>
+      <c r="D207" s="61"/>
+      <c r="E207" s="61"/>
+      <c r="F207" s="61"/>
+      <c r="G207" s="61"/>
       <c r="H207" s="1"/>
       <c r="I207" s="1"/>
       <c r="J207" s="1"/>
@@ -15833,14 +15745,14 @@
     </row>
     <row r="215" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1"/>
-      <c r="B215" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="C215" s="47"/>
-      <c r="D215" s="47"/>
-      <c r="E215" s="47"/>
-      <c r="F215" s="47"/>
-      <c r="G215" s="47"/>
+      <c r="B215" s="100" t="s">
+        <v>123</v>
+      </c>
+      <c r="C215" s="61"/>
+      <c r="D215" s="61"/>
+      <c r="E215" s="61"/>
+      <c r="F215" s="61"/>
+      <c r="G215" s="61"/>
       <c r="H215" s="1"/>
       <c r="I215" s="1"/>
       <c r="J215" s="1"/>
@@ -15863,12 +15775,12 @@
     </row>
     <row r="216" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1"/>
-      <c r="B216" s="47"/>
-      <c r="C216" s="47"/>
-      <c r="D216" s="47"/>
-      <c r="E216" s="47"/>
-      <c r="F216" s="47"/>
-      <c r="G216" s="47"/>
+      <c r="B216" s="61"/>
+      <c r="C216" s="61"/>
+      <c r="D216" s="61"/>
+      <c r="E216" s="61"/>
+      <c r="F216" s="61"/>
+      <c r="G216" s="61"/>
       <c r="H216" s="1"/>
       <c r="I216" s="1"/>
       <c r="J216" s="1"/>
@@ -38150,74 +38062,117 @@
       <c r="Z1011" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="202">
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="G78:G79"/>
-    <mergeCell ref="H78:H79"/>
-    <mergeCell ref="I78:I79"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="H82:H83"/>
-    <mergeCell ref="B84:G84"/>
-    <mergeCell ref="B78:D79"/>
-    <mergeCell ref="B80:D81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="F80:F81"/>
-    <mergeCell ref="G80:G81"/>
-    <mergeCell ref="K70:M70"/>
-    <mergeCell ref="K71:M71"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="B74:I74"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="K65:M65"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="K66:M66"/>
-    <mergeCell ref="K67:M67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="K69:M69"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="E65:F65"/>
+  <mergeCells count="198">
+    <mergeCell ref="H80:H81"/>
+    <mergeCell ref="B82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="H168:N168"/>
+    <mergeCell ref="H173:I173"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B192:D192"/>
+    <mergeCell ref="B205:D205"/>
+    <mergeCell ref="B206:G207"/>
+    <mergeCell ref="B215:G216"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:D123"/>
+    <mergeCell ref="H130:M130"/>
+    <mergeCell ref="H157:M159"/>
+    <mergeCell ref="H142:M142"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="B11:D12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="B26:H26"/>
@@ -38240,122 +38195,152 @@
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B11:D12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H173:I173"/>
-    <mergeCell ref="H177:J177"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B192:D192"/>
-    <mergeCell ref="B205:D205"/>
-    <mergeCell ref="B206:G207"/>
-    <mergeCell ref="B215:G216"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:D123"/>
-    <mergeCell ref="H130:M130"/>
-    <mergeCell ref="H157:M159"/>
-    <mergeCell ref="H142:M142"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="H168:N168"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="I80:I81"/>
-    <mergeCell ref="H80:H81"/>
-    <mergeCell ref="B82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="K65:M65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="K67:M67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="K68:M68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="K69:M69"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="K70:M70"/>
+    <mergeCell ref="K71:M71"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B74:I74"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="H82:H83"/>
+    <mergeCell ref="B84:G84"/>
+    <mergeCell ref="B78:D79"/>
+    <mergeCell ref="B80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="F80:F81"/>
+    <mergeCell ref="G80:G81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E013306-B5FA-4E65-BB14-0D10D59FC3FB}">
+  <dimension ref="H1:K6"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="8:11" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="8:11" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H3" s="116" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="117" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="117" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H4" s="118" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="119" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="119" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="119" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H5" s="120">
+        <f>-('Viabilidad economica'!E118)</f>
+        <v>-14877.357002999999</v>
+      </c>
+      <c r="I5" s="121">
+        <f>'Viabilidad economica'!F118</f>
+        <v>15421.714895999999</v>
+      </c>
+      <c r="J5" s="121">
+        <f>'Viabilidad economica'!G118</f>
+        <v>15421.714895999999</v>
+      </c>
+      <c r="K5" s="121">
+        <f>'Viabilidad economica'!H118</f>
+        <v>15421.714895999999</v>
+      </c>
+    </row>
+    <row r="6" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H6" s="122" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6" s="123"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="125">
+        <f>IRR(H5:K5)</f>
+        <v>0.88078075152630331</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H6:J6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>